<commit_message>
git commit -m "test data file is modifidf
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D927A8E-81BC-48DF-A7BA-B4315B60E0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1FF63C-19B5-4090-888C-FF0BDE72AB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="392">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1183,15 +1183,6 @@
     <t>Wilson41</t>
   </si>
   <si>
-    <t>Patric42</t>
-  </si>
-  <si>
-    <t>Wilson42</t>
-  </si>
-  <si>
-    <t>ssr42@gmail.com</t>
-  </si>
-  <si>
     <t>ssr44@gmail.com</t>
   </si>
   <si>
@@ -1201,22 +1192,13 @@
     <t>Wilson44</t>
   </si>
   <si>
-    <t>ssr46@gmail.com</t>
-  </si>
-  <si>
     <t>ssr47@gmail.com</t>
   </si>
   <si>
     <t>Event Created By Automation7</t>
   </si>
   <si>
-    <t>EventAutomation8</t>
-  </si>
-  <si>
     <t>EventAutomation9</t>
-  </si>
-  <si>
-    <t>http://www.myevents.com/automationevent987899</t>
   </si>
   <si>
     <t>http://www.myevents.com/automationevent9878999</t>
@@ -1429,17 +1411,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1447,17 +1423,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1768,7 +1750,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -1782,7 +1764,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -1942,13 +1924,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="41"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="41"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1961,7 +1943,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2228,7 +2210,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="42"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2261,7 +2243,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="42"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -2606,14 +2588,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3151,13 +3133,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3185,13 +3167,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3219,6 +3201,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3235,11 +3222,6 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3345,9 +3327,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE47"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -3396,13 +3378,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
+        <v>385</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>387</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>386</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -3416,50 +3398,50 @@
       <c r="G2" s="36" t="s">
         <v>382</v>
       </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>388</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>382</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="23"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="15"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -3473,10 +3455,11 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="23"/>
+      <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="23"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
@@ -3598,75 +3581,67 @@
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-    </row>
-    <row r="12" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="16"/>
-    </row>
-    <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
+    <row r="11" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="16"/>
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
@@ -3684,125 +3659,128 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="17"/>
-      <c r="AA16" s="19"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="19"/>
-      <c r="AE16" s="16"/>
-    </row>
-    <row r="17" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="20"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-    </row>
-    <row r="20" spans="2:31" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-    </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="16"/>
+    </row>
+    <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+    </row>
+    <row r="19" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="15"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
-      <c r="Q21" s="23"/>
+      <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3821,7 +3799,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -3840,15 +3818,15 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -3859,15 +3837,15 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -3878,14 +3856,14 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+    <row r="26" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -3897,7 +3875,7 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -3916,52 +3894,52 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+    <row r="28" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+    <row r="29" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+    <row r="30" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -3973,41 +3951,41 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+    <row r="31" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
     </row>
-    <row r="32" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+    <row r="32" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="35"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
     </row>
@@ -4021,7 +3999,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="35"/>
+      <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
@@ -4031,40 +4009,40 @@
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="35"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
     </row>
@@ -4078,7 +4056,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="35"/>
+      <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
@@ -4088,54 +4066,54 @@
       <c r="R36" s="6"/>
     </row>
     <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
     </row>
     <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="35"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-      <c r="K39" s="35"/>
+      <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
@@ -4163,7 +4141,7 @@
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
@@ -4209,16 +4187,6 @@
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
@@ -4247,29 +4215,19 @@
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1E72998F-D12D-4ABD-9FF6-632927FA01A4}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -4312,8 +4270,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>391</v>
+      <c r="A2" s="33" t="s">
+        <v>388</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>383</v>
@@ -4337,36 +4295,9 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>392</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>382</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{23449C0A-3E4C-4892-9DF2-9181A0499BB2}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4401,9 +4332,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -4427,30 +4358,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{D3B9450A-B03E-4978-864F-767D2F738B12}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5127,7 +5046,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5183,7 +5102,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -5327,7 +5246,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="37" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -5338,7 +5257,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="45" t="s">
+      <c r="F30" s="46" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -5370,7 +5289,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -5379,7 +5298,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="45"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -5419,7 +5338,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="45" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -5440,7 +5359,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="44" t="s">
+      <c r="K33" s="45" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -5460,7 +5379,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -5479,7 +5398,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="44"/>
+      <c r="K34" s="45"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -5500,7 +5419,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="45" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -5521,7 +5440,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="44" t="s">
+      <c r="K36" s="45" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -5541,7 +5460,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -5560,7 +5479,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="44"/>
+      <c r="K37" s="45"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -5578,7 +5497,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="46" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -5596,7 +5515,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="44" t="s">
+      <c r="K39" s="45" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -5616,7 +5535,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -5632,7 +5551,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="44"/>
+      <c r="K40" s="45"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -5650,7 +5569,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="37" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -5685,7 +5604,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -5730,7 +5649,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="42" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5783,7 +5702,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="39"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -5834,7 +5753,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="37" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -5899,7 +5818,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -5963,11 +5882,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -5977,6 +5891,11 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
test data is moified
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1FF63C-19B5-4090-888C-FF0BDE72AB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7227403D-4D78-44E1-9409-2C20BAC30EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1183,18 +1183,12 @@
     <t>Wilson41</t>
   </si>
   <si>
-    <t>ssr44@gmail.com</t>
-  </si>
-  <si>
     <t>Patric44</t>
   </si>
   <si>
     <t>Wilson44</t>
   </si>
   <si>
-    <t>ssr47@gmail.com</t>
-  </si>
-  <si>
     <t>Event Created By Automation7</t>
   </si>
   <si>
@@ -1202,6 +1196,12 @@
   </si>
   <si>
     <t>http://www.myevents.com/automationevent9878999</t>
+  </si>
+  <si>
+    <t>ssr51@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr52@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -3329,8 +3329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3378,13 +3378,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>386</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>387</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -4218,7 +4218,7 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F04E53C0-2E63-4EE9-B7F0-5AECA9291772}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -4229,8 +4229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>383</v>
@@ -4297,7 +4297,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1FE916CF-5362-48A7-B84A-0E6E7E90D1F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4358,13 +4358,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>389</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test data modified  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7227403D-4D78-44E1-9409-2C20BAC30EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9965E0-7D0A-4D80-90AC-A473F88E54A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1189,19 +1189,19 @@
     <t>Wilson44</t>
   </si>
   <si>
-    <t>Event Created By Automation7</t>
-  </si>
-  <si>
-    <t>EventAutomation9</t>
-  </si>
-  <si>
-    <t>http://www.myevents.com/automationevent9878999</t>
-  </si>
-  <si>
     <t>ssr51@gmail.com</t>
   </si>
   <si>
     <t>ssr52@gmail.com</t>
+  </si>
+  <si>
+    <t>EventAutomation19</t>
+  </si>
+  <si>
+    <t>Event Created By Automation17</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789999</t>
   </si>
 </sst>
 </file>
@@ -1411,11 +1411,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1423,23 +1429,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1750,7 +1750,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -1764,7 +1764,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -1924,13 +1924,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="37"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="37"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1943,7 +1943,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2210,7 +2210,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="39"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2243,7 +2243,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="39"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -2588,14 +2588,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3133,13 +3133,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="42"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3167,13 +3167,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
+      <c r="B61" s="41"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3201,11 +3201,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3222,6 +3217,11 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>385</v>
@@ -4229,7 +4229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>383</v>
@@ -4334,8 +4334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,18 +4358,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B2" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{93D1F61C-96E2-42D1-B1CC-0BD9A62A9760}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5046,7 +5046,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="46" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5102,7 +5102,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -5246,7 +5246,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="40" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="45" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -5289,7 +5289,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="46"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -5338,7 +5338,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="44" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -5359,7 +5359,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="45" t="s">
+      <c r="K33" s="44" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -5379,7 +5379,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -5398,7 +5398,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="45"/>
+      <c r="K34" s="44"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -5419,7 +5419,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="44" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -5440,7 +5440,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="45" t="s">
+      <c r="K36" s="44" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -5460,7 +5460,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -5479,7 +5479,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="45"/>
+      <c r="K37" s="44"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -5497,7 +5497,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="45" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -5515,7 +5515,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="45" t="s">
+      <c r="K39" s="44" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -5535,7 +5535,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -5551,7 +5551,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="45"/>
+      <c r="K40" s="44"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -5569,7 +5569,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="40" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -5604,7 +5604,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -5649,7 +5649,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="39" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5702,7 +5702,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -5753,7 +5753,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="40" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -5818,7 +5818,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -5882,6 +5882,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -5891,11 +5896,6 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
New Test data file created
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9965E0-7D0A-4D80-90AC-A473F88E54A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D927A8E-81BC-48DF-A7BA-B4315B60E0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="398">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1183,25 +1183,43 @@
     <t>Wilson41</t>
   </si>
   <si>
+    <t>Patric42</t>
+  </si>
+  <si>
+    <t>Wilson42</t>
+  </si>
+  <si>
+    <t>ssr42@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr44@gmail.com</t>
+  </si>
+  <si>
     <t>Patric44</t>
   </si>
   <si>
     <t>Wilson44</t>
   </si>
   <si>
-    <t>ssr51@gmail.com</t>
-  </si>
-  <si>
-    <t>ssr52@gmail.com</t>
-  </si>
-  <si>
-    <t>EventAutomation19</t>
-  </si>
-  <si>
-    <t>Event Created By Automation17</t>
-  </si>
-  <si>
-    <t>http://www.myevents.com/automationevent98789999</t>
+    <t>ssr46@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr47@gmail.com</t>
+  </si>
+  <si>
+    <t>Event Created By Automation7</t>
+  </si>
+  <si>
+    <t>EventAutomation8</t>
+  </si>
+  <si>
+    <t>EventAutomation9</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent987899</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent9878999</t>
   </si>
 </sst>
 </file>
@@ -3327,10 +3345,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE46"/>
+  <dimension ref="A1:AE47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,50 +3416,50 @@
       <c r="G2" s="36" t="s">
         <v>382</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="23"/>
+      <c r="A3" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -3455,11 +3473,10 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
+      <c r="S4" s="23"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
+      <c r="V4" s="23"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
@@ -3581,67 +3598,75 @@
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="16"/>
-    </row>
-    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="16"/>
+    </row>
+    <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
@@ -3659,128 +3684,125 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="17"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="13"/>
-      <c r="AD15" s="19"/>
-      <c r="AE15" s="16"/>
-    </row>
-    <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-    </row>
-    <row r="19" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="19"/>
+      <c r="AE16" s="16"/>
+    </row>
+    <row r="17" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+    </row>
+    <row r="20" spans="2:31" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="K21" s="15"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
+      <c r="Q21" s="23"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3799,7 +3821,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -3818,15 +3840,15 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -3837,15 +3859,15 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -3856,14 +3878,14 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -3875,7 +3897,7 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -3894,52 +3916,52 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+    <row r="28" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+    <row r="29" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
+    <row r="30" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -3951,41 +3973,41 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="6"/>
+    <row r="31" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
     </row>
-    <row r="32" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+    <row r="32" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="35"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
     </row>
@@ -3999,7 +4021,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
+      <c r="K33" s="35"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
@@ -4009,40 +4031,40 @@
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="35"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
     </row>
@@ -4056,7 +4078,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="K36" s="35"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
@@ -4066,54 +4088,54 @@
       <c r="R36" s="6"/>
     </row>
     <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
     </row>
     <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="35"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="K39" s="35"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
@@ -4141,7 +4163,7 @@
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
@@ -4187,6 +4209,16 @@
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
@@ -4215,22 +4247,32 @@
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
     </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F04E53C0-2E63-4EE9-B7F0-5AECA9291772}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1E72998F-D12D-4ABD-9FF6-632927FA01A4}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4270,8 +4312,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>388</v>
+      <c r="A2" s="23" t="s">
+        <v>391</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>383</v>
@@ -4295,9 +4337,36 @@
         <v>382</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1FE916CF-5362-48A7-B84A-0E6E7E90D1F7}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{23449C0A-3E4C-4892-9DF2-9181A0499BB2}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4332,10 +4401,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,18 +4427,30 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B2" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>391</v>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{93D1F61C-96E2-42D1-B1CC-0BD9A62A9760}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D3B9450A-B03E-4978-864F-767D2F738B12}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Test data file created with new data
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D927A8E-81BC-48DF-A7BA-B4315B60E0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52202DB5-1DF2-4008-9D57-A673DBDC35AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="400">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1183,15 +1183,6 @@
     <t>Wilson41</t>
   </si>
   <si>
-    <t>Patric42</t>
-  </si>
-  <si>
-    <t>Wilson42</t>
-  </si>
-  <si>
-    <t>ssr42@gmail.com</t>
-  </si>
-  <si>
     <t>ssr44@gmail.com</t>
   </si>
   <si>
@@ -1201,25 +1192,40 @@
     <t>Wilson44</t>
   </si>
   <si>
-    <t>ssr46@gmail.com</t>
-  </si>
-  <si>
     <t>ssr47@gmail.com</t>
   </si>
   <si>
     <t>Event Created By Automation7</t>
   </si>
   <si>
-    <t>EventAutomation8</t>
-  </si>
-  <si>
     <t>EventAutomation9</t>
   </si>
   <si>
-    <t>http://www.myevents.com/automationevent987899</t>
-  </si>
-  <si>
     <t>http://www.myevents.com/automationevent9878999</t>
+  </si>
+  <si>
+    <t>ssr62@gmail.com</t>
+  </si>
+  <si>
+    <t>Patric62</t>
+  </si>
+  <si>
+    <t>Wilson62</t>
+  </si>
+  <si>
+    <t>ssr66@gmail.com</t>
+  </si>
+  <si>
+    <t>Patric46</t>
+  </si>
+  <si>
+    <t>Wilson46</t>
+  </si>
+  <si>
+    <t>EventAutomation18</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789918</t>
   </si>
 </sst>
 </file>
@@ -1429,17 +1435,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1447,17 +1447,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1768,7 +1774,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -1782,7 +1788,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -1942,13 +1948,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="41"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="41"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1961,7 +1967,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2228,7 +2234,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="42"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2261,7 +2267,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="42"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -2606,14 +2612,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3151,13 +3157,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3185,13 +3191,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3219,6 +3225,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3235,11 +3246,6 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3348,7 +3354,7 @@
   <dimension ref="A1:AE47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,13 +3402,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -3419,13 +3425,13 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>358</v>
@@ -4259,8 +4265,8 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1E72998F-D12D-4ABD-9FF6-632927FA01A4}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{EF1677DB-B4E5-415A-B214-1670D5524E0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4272,7 +4278,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4312,14 +4318,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>391</v>
+      <c r="A2" s="33" t="s">
+        <v>395</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -4339,7 +4345,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>383</v>
@@ -4365,8 +4371,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{23449C0A-3E4C-4892-9DF2-9181A0499BB2}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{250C0EFC-F392-4631-82E9-0E13160B607B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4404,7 +4410,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4427,30 +4433,30 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{D3B9450A-B03E-4978-864F-767D2F738B12}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{619D9C47-A3C4-4E0C-9C2E-028A7877C1AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5127,7 +5133,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5183,7 +5189,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -5327,7 +5333,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="37" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -5338,7 +5344,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="45" t="s">
+      <c r="F30" s="46" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -5370,7 +5376,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -5379,7 +5385,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="45"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -5419,7 +5425,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="45" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -5440,7 +5446,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="44" t="s">
+      <c r="K33" s="45" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -5460,7 +5466,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -5479,7 +5485,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="44"/>
+      <c r="K34" s="45"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -5500,7 +5506,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="45" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -5521,7 +5527,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="44" t="s">
+      <c r="K36" s="45" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -5541,7 +5547,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -5560,7 +5566,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="44"/>
+      <c r="K37" s="45"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -5578,7 +5584,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="46" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -5596,7 +5602,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="44" t="s">
+      <c r="K39" s="45" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -5616,7 +5622,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -5632,7 +5638,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="44"/>
+      <c r="K40" s="45"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -5650,7 +5656,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="37" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -5685,7 +5691,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -5730,7 +5736,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="42" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5783,7 +5789,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="39"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -5834,7 +5840,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="37" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -5899,7 +5905,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -5963,11 +5969,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -5977,6 +5978,11 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
New Test Data added
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52202DB5-1DF2-4008-9D57-A673DBDC35AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DA30F0-30A6-46E9-BB79-E9AF6F08480F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="575">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1177,55 +1177,580 @@
     <t>  Chicago</t>
   </si>
   <si>
-    <t>Patric41</t>
-  </si>
-  <si>
-    <t>Wilson41</t>
-  </si>
-  <si>
-    <t>ssr44@gmail.com</t>
-  </si>
-  <si>
-    <t>Patric44</t>
-  </si>
-  <si>
-    <t>Wilson44</t>
-  </si>
-  <si>
-    <t>ssr47@gmail.com</t>
-  </si>
-  <si>
-    <t>Event Created By Automation7</t>
-  </si>
-  <si>
-    <t>EventAutomation9</t>
-  </si>
-  <si>
-    <t>http://www.myevents.com/automationevent9878999</t>
-  </si>
-  <si>
     <t>ssr62@gmail.com</t>
   </si>
   <si>
     <t>Patric62</t>
   </si>
   <si>
+    <t>ssr66@gmail.com</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789918</t>
+  </si>
+  <si>
+    <t>Wilson63</t>
+  </si>
+  <si>
     <t>Wilson62</t>
   </si>
   <si>
-    <t>ssr66@gmail.com</t>
-  </si>
-  <si>
-    <t>Patric46</t>
-  </si>
-  <si>
-    <t>Wilson46</t>
-  </si>
-  <si>
-    <t>EventAutomation18</t>
-  </si>
-  <si>
-    <t>http://www.myevents.com/automationevent98789918</t>
+    <t>Patric63</t>
+  </si>
+  <si>
+    <t>Patric64</t>
+  </si>
+  <si>
+    <t>Patric65</t>
+  </si>
+  <si>
+    <t>Patric66</t>
+  </si>
+  <si>
+    <t>Patric67</t>
+  </si>
+  <si>
+    <t>Patric68</t>
+  </si>
+  <si>
+    <t>Patric69</t>
+  </si>
+  <si>
+    <t>Patric70</t>
+  </si>
+  <si>
+    <t>Patric71</t>
+  </si>
+  <si>
+    <t>Patric72</t>
+  </si>
+  <si>
+    <t>Patric73</t>
+  </si>
+  <si>
+    <t>Patric74</t>
+  </si>
+  <si>
+    <t>Patric75</t>
+  </si>
+  <si>
+    <t>Patric76</t>
+  </si>
+  <si>
+    <t>Patric77</t>
+  </si>
+  <si>
+    <t>Patric78</t>
+  </si>
+  <si>
+    <t>Patric79</t>
+  </si>
+  <si>
+    <t>Wilson64</t>
+  </si>
+  <si>
+    <t>Wilson65</t>
+  </si>
+  <si>
+    <t>Wilson66</t>
+  </si>
+  <si>
+    <t>Wilson67</t>
+  </si>
+  <si>
+    <t>Wilson68</t>
+  </si>
+  <si>
+    <t>Wilson69</t>
+  </si>
+  <si>
+    <t>Wilson70</t>
+  </si>
+  <si>
+    <t>Wilson71</t>
+  </si>
+  <si>
+    <t>Wilson72</t>
+  </si>
+  <si>
+    <t>Wilson73</t>
+  </si>
+  <si>
+    <t>Wilson74</t>
+  </si>
+  <si>
+    <t>Wilson75</t>
+  </si>
+  <si>
+    <t>Wilson76</t>
+  </si>
+  <si>
+    <t>Wilson77</t>
+  </si>
+  <si>
+    <t>Wilson78</t>
+  </si>
+  <si>
+    <t>Wilson79</t>
+  </si>
+  <si>
+    <t>ssr63@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr64@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr65@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr67@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr68@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr69@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr70@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr71@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr72@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr73@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr74@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr75@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr76@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr77@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr78@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr79@gmail.com</t>
+  </si>
+  <si>
+    <t>Patric80</t>
+  </si>
+  <si>
+    <t>Wilson80</t>
+  </si>
+  <si>
+    <t>Patric81</t>
+  </si>
+  <si>
+    <t>Wilson81</t>
+  </si>
+  <si>
+    <t>Patric82</t>
+  </si>
+  <si>
+    <t>Wilson82</t>
+  </si>
+  <si>
+    <t>Patric83</t>
+  </si>
+  <si>
+    <t>Wilson83</t>
+  </si>
+  <si>
+    <t>Patric84</t>
+  </si>
+  <si>
+    <t>Wilson84</t>
+  </si>
+  <si>
+    <t>Patric85</t>
+  </si>
+  <si>
+    <t>Wilson85</t>
+  </si>
+  <si>
+    <t>Patric86</t>
+  </si>
+  <si>
+    <t>Wilson86</t>
+  </si>
+  <si>
+    <t>Patric87</t>
+  </si>
+  <si>
+    <t>Wilson87</t>
+  </si>
+  <si>
+    <t>Patric88</t>
+  </si>
+  <si>
+    <t>Wilson88</t>
+  </si>
+  <si>
+    <t>Patric89</t>
+  </si>
+  <si>
+    <t>Wilson89</t>
+  </si>
+  <si>
+    <t>Patric90</t>
+  </si>
+  <si>
+    <t>Wilson90</t>
+  </si>
+  <si>
+    <t>Patric91</t>
+  </si>
+  <si>
+    <t>Wilson91</t>
+  </si>
+  <si>
+    <t>Patric92</t>
+  </si>
+  <si>
+    <t>Wilson92</t>
+  </si>
+  <si>
+    <t>Patric93</t>
+  </si>
+  <si>
+    <t>Wilson93</t>
+  </si>
+  <si>
+    <t>Patric94</t>
+  </si>
+  <si>
+    <t>Wilson94</t>
+  </si>
+  <si>
+    <t>Patric95</t>
+  </si>
+  <si>
+    <t>Wilson95</t>
+  </si>
+  <si>
+    <t>Patric96</t>
+  </si>
+  <si>
+    <t>Wilson96</t>
+  </si>
+  <si>
+    <t>Patric97</t>
+  </si>
+  <si>
+    <t>Wilson97</t>
+  </si>
+  <si>
+    <t>Patric98</t>
+  </si>
+  <si>
+    <t>Wilson98</t>
+  </si>
+  <si>
+    <t>Patric99</t>
+  </si>
+  <si>
+    <t>Wilson99</t>
+  </si>
+  <si>
+    <t>Patric100</t>
+  </si>
+  <si>
+    <t>Wilson100</t>
+  </si>
+  <si>
+    <t>Patric101</t>
+  </si>
+  <si>
+    <t>Wilson101</t>
+  </si>
+  <si>
+    <t>Patric102</t>
+  </si>
+  <si>
+    <t>Wilson102</t>
+  </si>
+  <si>
+    <t>Patric103</t>
+  </si>
+  <si>
+    <t>Wilson103</t>
+  </si>
+  <si>
+    <t>ssr80@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr81@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr82@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr83@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr84@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr85@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr86@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr87@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr88@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr89@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr90@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr91@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr92@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr93@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr94@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr95@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr96@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr97@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr98@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr99@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr100@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr101@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr102@gmail.com</t>
+  </si>
+  <si>
+    <t>ssr103@gmail.com</t>
+  </si>
+  <si>
+    <t>EventAutomation30</t>
+  </si>
+  <si>
+    <t>EventAutomation31</t>
+  </si>
+  <si>
+    <t>EventAutomation32</t>
+  </si>
+  <si>
+    <t>EventAutomation33</t>
+  </si>
+  <si>
+    <t>EventAutomation34</t>
+  </si>
+  <si>
+    <t>EventAutomation35</t>
+  </si>
+  <si>
+    <t>EventAutomation36</t>
+  </si>
+  <si>
+    <t>EventAutomation37</t>
+  </si>
+  <si>
+    <t>EventAutomation38</t>
+  </si>
+  <si>
+    <t>EventAutomation39</t>
+  </si>
+  <si>
+    <t>EventAutomation40</t>
+  </si>
+  <si>
+    <t>EventAutomation41</t>
+  </si>
+  <si>
+    <t>EventAutomation42</t>
+  </si>
+  <si>
+    <t>EventAutomation43</t>
+  </si>
+  <si>
+    <t>EventAutomation44</t>
+  </si>
+  <si>
+    <t>EventAutomation45</t>
+  </si>
+  <si>
+    <t>EventAutomation46</t>
+  </si>
+  <si>
+    <t>EventAutomation47</t>
+  </si>
+  <si>
+    <t>EventAutomation48</t>
+  </si>
+  <si>
+    <t>EventAutomation49</t>
+  </si>
+  <si>
+    <t>EventAutomation50</t>
+  </si>
+  <si>
+    <t>EventAutomation51</t>
+  </si>
+  <si>
+    <t>Event Created By Automation30</t>
+  </si>
+  <si>
+    <t>Event Created By Automation32</t>
+  </si>
+  <si>
+    <t>Event Created By Automation33</t>
+  </si>
+  <si>
+    <t>Event Created By Automation34</t>
+  </si>
+  <si>
+    <t>Event Created By Automation35</t>
+  </si>
+  <si>
+    <t>Event Created By Automation36</t>
+  </si>
+  <si>
+    <t>Event Created By Automation37</t>
+  </si>
+  <si>
+    <t>Event Created By Automation38</t>
+  </si>
+  <si>
+    <t>Event Created By Automation39</t>
+  </si>
+  <si>
+    <t>Event Created By Automation40</t>
+  </si>
+  <si>
+    <t>Event Created By Automation41</t>
+  </si>
+  <si>
+    <t>Event Created By Automation42</t>
+  </si>
+  <si>
+    <t>Event Created By Automation43</t>
+  </si>
+  <si>
+    <t>Event Created By Automation44</t>
+  </si>
+  <si>
+    <t>Event Created By Automation45</t>
+  </si>
+  <si>
+    <t>Event Created By Automation46</t>
+  </si>
+  <si>
+    <t>Event Created By Automation47</t>
+  </si>
+  <si>
+    <t>Event Created By Automation48</t>
+  </si>
+  <si>
+    <t>Event Created By Automation49</t>
+  </si>
+  <si>
+    <t>Event Created By Automation50</t>
+  </si>
+  <si>
+    <t>Event Created By Automation51</t>
+  </si>
+  <si>
+    <t>Event Created By Automation31</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789919</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789920</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789921</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789922</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789923</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789924</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789925</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789926</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789927</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789928</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789929</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789930</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789931</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789932</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789933</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789934</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789935</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789936</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789937</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789938</t>
+  </si>
+  <si>
+    <t>http://www.myevents.com/automationevent98789939</t>
   </si>
 </sst>
 </file>
@@ -1363,7 +1888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1435,11 +1960,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1447,23 +1979,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1774,7 +2300,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -1788,7 +2314,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -1948,13 +2474,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="38"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="38"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1967,7 +2493,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2234,7 +2760,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="40"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2267,7 +2793,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="40"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -2612,14 +3138,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -2647,13 +3173,13 @@
     </row>
     <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -2681,13 +3207,13 @@
     </row>
     <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2715,13 +3241,13 @@
     </row>
     <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -2749,13 +3275,13 @@
     </row>
     <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -2783,13 +3309,13 @@
     </row>
     <row r="49" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -2817,13 +3343,13 @@
     </row>
     <row r="50" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -2851,13 +3377,13 @@
     </row>
     <row r="51" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -2885,13 +3411,13 @@
     </row>
     <row r="52" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -2919,13 +3445,13 @@
     </row>
     <row r="53" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -2953,13 +3479,13 @@
     </row>
     <row r="54" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -3021,13 +3547,13 @@
     </row>
     <row r="56" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="38"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3055,13 +3581,13 @@
     </row>
     <row r="57" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="38"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -3089,13 +3615,13 @@
     </row>
     <row r="58" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -3123,13 +3649,13 @@
     </row>
     <row r="59" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -3157,13 +3683,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3191,13 +3717,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3225,11 +3751,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3246,6 +3767,11 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3354,7 +3880,7 @@
   <dimension ref="A1:AE47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,14 +3927,14 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>392</v>
+      <c r="A2" s="37" t="s">
+        <v>383</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -3424,11 +3950,11 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>385</v>
+      <c r="A3" s="37" t="s">
+        <v>422</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>387</v>
@@ -3462,12 +3988,27 @@
       <c r="V3" s="8"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="A4" s="37" t="s">
+        <v>423</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -3485,12 +4026,27 @@
       <c r="V4" s="23"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="A5" s="37" t="s">
+        <v>424</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -3509,12 +4065,27 @@
       <c r="W5" s="6"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="37" t="s">
+        <v>385</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -3533,12 +4104,27 @@
       <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="A7" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -3557,12 +4143,27 @@
       <c r="W7" s="6"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="A8" s="37" t="s">
+        <v>426</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -3581,12 +4182,27 @@
       <c r="W8" s="6"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -3605,12 +4221,27 @@
       <c r="W9" s="6"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="37" t="s">
+        <v>428</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -3628,13 +4259,51 @@
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
     </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>429</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
     <row r="12" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="A12" s="37" t="s">
+        <v>430</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -3652,12 +4321,27 @@
       <c r="V12" s="16"/>
     </row>
     <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="20"/>
+      <c r="A13" s="37" t="s">
+        <v>431</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
@@ -3675,12 +4359,27 @@
       <c r="V13" s="6"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="A14" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -3691,12 +4390,27 @@
       <c r="O14" s="6"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -3707,12 +4421,27 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="A16" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -3738,13 +4467,28 @@
       <c r="AD16" s="19"/>
       <c r="AE16" s="16"/>
     </row>
-    <row r="17" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="6"/>
+    <row r="17" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>435</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>382</v>
+      </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -3770,7 +4514,53 @@
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
     </row>
-    <row r="20" spans="2:31" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
@@ -3789,7 +4579,7 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -3808,7 +4598,7 @@
       <c r="Q21" s="23"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3827,7 +4617,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -3846,7 +4636,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -3865,7 +4655,7 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -3884,7 +4674,7 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -3903,7 +4693,7 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -3922,7 +4712,7 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
@@ -3941,7 +4731,7 @@
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="27"/>
@@ -3960,7 +4750,7 @@
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="27"/>
@@ -3979,7 +4769,7 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
@@ -3998,7 +4788,7 @@
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
     </row>
-    <row r="32" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="1"/>
@@ -4264,21 +5054,17 @@
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{35CA1DAD-660B-453C-9A6E-255AD1E77359}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{EF1677DB-B4E5-415A-B214-1670D5524E0D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,14 +5104,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>395</v>
+      <c r="A2" s="37" t="s">
+        <v>486</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>396</v>
+        <v>438</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>397</v>
+        <v>439</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -4344,14 +5130,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>388</v>
+      <c r="A3" s="37" t="s">
+        <v>487</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>383</v>
+        <v>440</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>384</v>
+        <v>441</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>358</v>
@@ -4369,11 +5155,580 @@
         <v>382</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>488</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>489</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>497</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>498</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>500</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>501</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>502</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>503</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>504</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>505</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
+        <v>506</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
+        <v>507</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>508</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>509</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>382</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{7A72A927-4BAB-4907-BD23-85281E06CB89}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{250C0EFC-F392-4631-82E9-0E13160B607B}"/>
-  </hyperlinks>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4407,16 +5762,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4433,30 +5788,251 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>398</v>
+        <v>510</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>532</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>390</v>
+        <v>511</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>553</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>391</v>
+        <v>554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B7" t="s">
+        <v>536</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B8" t="s">
+        <v>537</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>517</v>
+      </c>
+      <c r="B9" t="s">
+        <v>538</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B10" t="s">
+        <v>539</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>519</v>
+      </c>
+      <c r="B11" t="s">
+        <v>540</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>520</v>
+      </c>
+      <c r="B12" t="s">
+        <v>541</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>521</v>
+      </c>
+      <c r="B13" t="s">
+        <v>542</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>522</v>
+      </c>
+      <c r="B14" t="s">
+        <v>543</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B15" t="s">
+        <v>544</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>524</v>
+      </c>
+      <c r="B16" t="s">
+        <v>545</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>525</v>
+      </c>
+      <c r="B17" t="s">
+        <v>546</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>526</v>
+      </c>
+      <c r="B18" t="s">
+        <v>547</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>527</v>
+      </c>
+      <c r="B19" t="s">
+        <v>548</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>528</v>
+      </c>
+      <c r="B20" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>529</v>
+      </c>
+      <c r="B21" t="s">
+        <v>550</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>530</v>
+      </c>
+      <c r="B22" t="s">
+        <v>551</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>531</v>
+      </c>
+      <c r="B23" t="s">
+        <v>552</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>574</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{36D916D7-1D27-4018-884C-6B577DE35246}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{619D9C47-A3C4-4E0C-9C2E-028A7877C1AE}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{619D9C47-A3C4-4E0C-9C2E-028A7877C1AE}"/>
+    <hyperlink ref="C3:C23" r:id="rId2" display="http://www.myevents.com/automationevent98789918" xr:uid="{35BDE04D-5D5D-4573-AFE2-F49301F62861}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4483,7 +6059,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -4587,7 +6163,7 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
+      <c r="A2" s="44"/>
       <c r="B2" s="6" t="s">
         <v>188</v>
       </c>
@@ -5133,7 +6709,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5189,7 +6765,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -5258,7 +6834,7 @@
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="44" t="s">
         <v>198</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -5290,7 +6866,7 @@
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="6" t="s">
         <v>203</v>
       </c>
@@ -5333,7 +6909,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="41" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -5376,7 +6952,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -5656,7 +7232,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="41" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -5691,7 +7267,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -5736,7 +7312,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="40" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5789,7 +7365,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -5840,7 +7416,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="41" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -5905,7 +7481,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -5969,6 +7545,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -5978,11 +7559,6 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
added create new form method
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A225A1AD-545E-41E8-8650-36ADDBFCF420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1144FE-5E9E-4D70-A7A1-003FB85213E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="CreateNewPage" sheetId="8" r:id="rId2"/>
     <sheet name="CreateUser" sheetId="2" r:id="rId3"/>
-    <sheet name="CreateTeamUser" sheetId="5" r:id="rId4"/>
-    <sheet name="SearchUser" sheetId="6" r:id="rId5"/>
-    <sheet name="NewEventDetails" sheetId="7" r:id="rId6"/>
-    <sheet name="Branch" sheetId="4" r:id="rId7"/>
+    <sheet name="CreateNewForm" sheetId="9" r:id="rId4"/>
+    <sheet name="CreateTeamUser" sheetId="5" r:id="rId5"/>
+    <sheet name="SearchUser" sheetId="6" r:id="rId6"/>
+    <sheet name="NewEventDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="Branch" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="569">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1682,6 +1683,57 @@
   </si>
   <si>
     <t>Automation13</t>
+  </si>
+  <si>
+    <t>FormTitle</t>
+  </si>
+  <si>
+    <t>FormDescription</t>
+  </si>
+  <si>
+    <t>FormSubmissionButtonText</t>
+  </si>
+  <si>
+    <t>FormPageURL</t>
+  </si>
+  <si>
+    <t>AutomationTesting</t>
+  </si>
+  <si>
+    <t>SubmitForm</t>
+  </si>
+  <si>
+    <t>AutoForm</t>
+  </si>
+  <si>
+    <t>EmailLabelNameStep2</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EmailIsRequire</t>
+  </si>
+  <si>
+    <t>CheckBoxLabelname</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>CheckboxIsRequired</t>
+  </si>
+  <si>
+    <t>CheckboxOption1</t>
+  </si>
+  <si>
+    <t>CheckboxOption2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -1819,7 +1871,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1892,11 +1944,17 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1904,23 +1962,20 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2231,7 +2286,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2245,7 +2300,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -2405,13 +2460,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="38"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="38"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2424,7 +2479,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2691,7 +2746,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
+      <c r="A32" s="40"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2724,7 +2779,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
+      <c r="A33" s="40"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3069,14 +3124,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3614,13 +3669,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3648,13 +3703,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3682,11 +3737,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3703,6 +3753,11 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3835,7 +3890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -4800,6 +4855,96 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2F08CA-A5DE-45FA-A34C-73FA0F2E9E41}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C2" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2" t="s">
+        <v>558</v>
+      </c>
+      <c r="E2" t="s">
+        <v>560</v>
+      </c>
+      <c r="F2" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>563</v>
+      </c>
+      <c r="H2" t="s">
+        <v>567</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -5369,7 +5514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76A90F2-FEBC-495D-96DD-9CDE989D1767}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5423,7 +5568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -5678,7 +5823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH52"/>
   <sheetViews>
@@ -6349,7 +6494,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -6405,7 +6550,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -6549,7 +6694,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="41" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6560,7 +6705,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="47" t="s">
+      <c r="F30" s="46" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6592,7 +6737,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6601,7 +6746,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="47"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6641,7 +6786,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="45" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6662,7 +6807,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="46" t="s">
+      <c r="K33" s="45" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6682,7 +6827,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6701,7 +6846,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="46"/>
+      <c r="K34" s="45"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6722,7 +6867,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="45" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6743,7 +6888,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="46" t="s">
+      <c r="K36" s="45" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6763,7 +6908,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6782,7 +6927,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="46"/>
+      <c r="K37" s="45"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6800,7 +6945,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="46" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6818,7 +6963,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="46" t="s">
+      <c r="K39" s="45" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6838,7 +6983,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6854,7 +6999,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="46"/>
+      <c r="K40" s="45"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6872,7 +7017,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="41" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6907,7 +7052,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6952,7 +7097,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="40" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -7005,7 +7150,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -7056,7 +7201,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="41" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -7121,7 +7266,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="38"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -7185,6 +7330,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -7194,11 +7344,6 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
added new code for unique user creation
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D19D0FE-E8E0-4BB2-9FB3-57B7A8297E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA67EA-607F-4A81-ADCA-5296A57DDFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="538">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1166,15 +1166,6 @@
     <t>Pre-Approved Page</t>
   </si>
   <si>
-    <t>Patric79</t>
-  </si>
-  <si>
-    <t>Wilson79</t>
-  </si>
-  <si>
-    <t>ssr79@gmail.com</t>
-  </si>
-  <si>
     <t>Patric94</t>
   </si>
   <si>
@@ -1514,9 +1505,6 @@
     <t>StatesofRegistrationFor DemoQA</t>
   </si>
   <si>
-    <t>98756327</t>
-  </si>
-  <si>
     <t>Patric80</t>
   </si>
   <si>
@@ -1625,9 +1613,6 @@
     <t>98756336</t>
   </si>
   <si>
-    <t>ssr80@gmail.com</t>
-  </si>
-  <si>
     <t>ssr81@gmail.com</t>
   </si>
   <si>
@@ -1653,6 +1638,9 @@
   </si>
   <si>
     <t>Alisha New</t>
+  </si>
+  <si>
+    <t>ssr80</t>
   </si>
 </sst>
 </file>
@@ -1873,17 +1861,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1891,17 +1873,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2212,7 +2200,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2226,7 +2214,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -2386,13 +2374,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="44"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2405,7 +2393,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2672,7 +2660,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="45"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2705,7 +2693,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="45"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3050,14 +3038,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3595,13 +3583,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3629,13 +3617,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3663,6 +3651,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3679,11 +3672,6 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3725,13 +3713,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>371</v>
@@ -3742,13 +3730,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E3" s="36"/>
       <c r="G3" s="36" t="s">
@@ -3757,13 +3745,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E4" s="36"/>
       <c r="G4" s="36" t="s">
@@ -3807,10 +3795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3851,7 +3839,7 @@
         <v>215</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>361</v>
@@ -3859,15 +3847,15 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>381</v>
+        <v>537</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>379</v>
+        <v>492</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>380</v>
+        <v>493</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -3876,18 +3864,28 @@
         <v>359</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>360</v>
+        <v>494</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>496</v>
@@ -3905,25 +3903,25 @@
         <v>498</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>500</v>
@@ -3941,25 +3939,25 @@
         <v>502</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>503</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="15"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
-      <c r="Q4" s="23"/>
+      <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>504</v>
@@ -3977,7 +3975,7 @@
         <v>506</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>507</v>
@@ -3995,7 +3993,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>508</v>
@@ -4013,7 +4011,7 @@
         <v>510</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>511</v>
@@ -4031,7 +4029,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>512</v>
@@ -4049,12 +4047,12 @@
         <v>514</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>515</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -4067,7 +4065,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>516</v>
@@ -4085,12 +4083,12 @@
         <v>518</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H8" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -4101,9 +4099,9 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>520</v>
@@ -4121,7 +4119,7 @@
         <v>522</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H9" s="20" t="s">
         <v>523</v>
@@ -4139,7 +4137,7 @@
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>524</v>
@@ -4157,7 +4155,7 @@
         <v>526</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H10" s="20" t="s">
         <v>527</v>
@@ -4174,68 +4172,51 @@
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>540</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>528</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>529</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>530</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>493</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>531</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -4248,40 +4229,40 @@
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="35"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
@@ -4295,7 +4276,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="35"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -4305,40 +4286,40 @@
       <c r="R16" s="6"/>
     </row>
     <row r="17" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
     <row r="18" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="35"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
     </row>
@@ -4352,7 +4333,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="35"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
@@ -4362,54 +4343,54 @@
       <c r="R19" s="6"/>
     </row>
     <row r="20" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
     </row>
     <row r="21" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="35"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
     </row>
     <row r="22" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="35"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -4437,7 +4418,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
@@ -4483,16 +4464,6 @@
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="27"/>
@@ -4520,15 +4491,6 @@
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -4559,63 +4521,63 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2" t="s">
         <v>463</v>
-      </c>
-      <c r="C2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D2" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2" t="s">
-        <v>466</v>
       </c>
       <c r="F2" s="38" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="H2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -4672,18 +4634,18 @@
         <v>215</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -4695,24 +4657,24 @@
         <v>360</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>358</v>
@@ -4724,24 +4686,24 @@
         <v>360</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>358</v>
@@ -4753,24 +4715,24 @@
         <v>360</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>358</v>
@@ -4782,24 +4744,24 @@
         <v>360</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>358</v>
@@ -4811,24 +4773,24 @@
         <v>360</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>358</v>
@@ -4840,24 +4802,24 @@
         <v>360</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>358</v>
@@ -4869,24 +4831,24 @@
         <v>360</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>358</v>
@@ -4898,24 +4860,24 @@
         <v>360</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>358</v>
@@ -4927,21 +4889,21 @@
         <v>360</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>358</v>
@@ -4953,10 +4915,10 @@
         <v>360</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -4985,33 +4947,33 @@
         <v>363</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="36" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="36" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="36" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -5024,7 +4986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -5048,145 +5010,145 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B7" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B9" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B11" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B13" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -5869,7 +5831,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5925,7 +5887,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -6069,7 +6031,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="40" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6080,7 +6042,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="49" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6112,7 +6074,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6121,7 +6083,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="48"/>
+      <c r="F31" s="49"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6161,7 +6123,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="48" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6182,7 +6144,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="47" t="s">
+      <c r="K33" s="48" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6202,7 +6164,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6221,7 +6183,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="47"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6242,7 +6204,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="48" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6263,7 +6225,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="47" t="s">
+      <c r="K36" s="48" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6283,7 +6245,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6302,7 +6264,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="47"/>
+      <c r="K37" s="48"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6320,7 +6282,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="49" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6338,7 +6300,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="47" t="s">
+      <c r="K39" s="48" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6358,7 +6320,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6374,7 +6336,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="47"/>
+      <c r="K40" s="48"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6392,7 +6354,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="40" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6427,7 +6389,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6472,7 +6434,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="45" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6525,7 +6487,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -6576,7 +6538,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="40" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6641,7 +6603,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -6705,11 +6667,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -6719,6 +6676,11 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
added code for test data with timestamp
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA67EA-607F-4A81-ADCA-5296A57DDFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A5A909-E574-4C46-B293-A5865722022C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="536">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1166,12 +1166,6 @@
     <t>Pre-Approved Page</t>
   </si>
   <si>
-    <t>Patric94</t>
-  </si>
-  <si>
-    <t>Wilson94</t>
-  </si>
-  <si>
     <t>Patric95</t>
   </si>
   <si>
@@ -1226,9 +1220,6 @@
     <t>Wilson103</t>
   </si>
   <si>
-    <t>ssr94@gmail.com</t>
-  </si>
-  <si>
     <t>ssr95@gmail.com</t>
   </si>
   <si>
@@ -1253,9 +1244,6 @@
     <t>ssr102@gmail.com</t>
   </si>
   <si>
-    <t>ssr103@gmail.com</t>
-  </si>
-  <si>
     <t>EventAutomation39</t>
   </si>
   <si>
@@ -1445,9 +1433,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>TestAutomation11</t>
-  </si>
-  <si>
     <t>TestAutomation12</t>
   </si>
   <si>
@@ -1505,12 +1490,6 @@
     <t>StatesofRegistrationFor DemoQA</t>
   </si>
   <si>
-    <t>Patric80</t>
-  </si>
-  <si>
-    <t>Wilson80</t>
-  </si>
-  <si>
     <t>853-046-6047</t>
   </si>
   <si>
@@ -1640,7 +1619,22 @@
     <t>Alisha New</t>
   </si>
   <si>
-    <t>ssr80</t>
+    <t>Patric</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>ssr</t>
+  </si>
+  <si>
+    <t>TestAutomation</t>
+  </si>
+  <si>
+    <t>tur</t>
+  </si>
+  <si>
+    <t>James</t>
   </si>
 </sst>
 </file>
@@ -1861,11 +1855,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1873,23 +1873,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2200,7 +2194,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2214,7 +2208,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
+      <c r="A2" s="43"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -2374,13 +2368,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="40"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2393,7 +2387,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2660,7 +2654,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="42"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2693,7 +2687,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="42"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3038,14 +3032,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3583,13 +3577,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3617,13 +3611,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3651,11 +3645,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3672,6 +3661,11 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -3713,13 +3707,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C2" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>371</v>
@@ -3730,13 +3724,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B3" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="E3" s="36"/>
       <c r="G3" s="36" t="s">
@@ -3745,13 +3739,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B4" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="E4" s="36"/>
       <c r="G4" s="36" t="s">
@@ -3797,8 +3791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3839,7 +3833,7 @@
         <v>215</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>361</v>
@@ -3849,13 +3843,13 @@
     </row>
     <row r="2" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>492</v>
+        <v>530</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>493</v>
+        <v>531</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -3864,13 +3858,13 @@
         <v>359</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
@@ -3885,13 +3879,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>358</v>
@@ -3900,13 +3894,13 @@
         <v>359</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -3921,13 +3915,13 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>358</v>
@@ -3936,13 +3930,13 @@
         <v>359</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -3957,13 +3951,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>358</v>
@@ -3972,13 +3966,13 @@
         <v>359</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -3993,13 +3987,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>358</v>
@@ -4008,13 +4002,13 @@
         <v>359</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -4029,13 +4023,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>358</v>
@@ -4044,13 +4038,13 @@
         <v>359</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="6"/>
@@ -4065,13 +4059,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>358</v>
@@ -4080,13 +4074,13 @@
         <v>359</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -4101,13 +4095,13 @@
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>358</v>
@@ -4116,13 +4110,13 @@
         <v>359</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -4137,13 +4131,13 @@
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>358</v>
@@ -4152,13 +4146,13 @@
         <v>359</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -4521,63 +4515,63 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>462</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>469</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D2" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="F2" s="38" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>462</v>
+      </c>
+      <c r="H2" t="s">
         <v>466</v>
       </c>
-      <c r="H2" t="s">
-        <v>470</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -4593,8 +4587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,18 +4628,18 @@
         <v>215</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>399</v>
+        <v>534</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>379</v>
+        <v>535</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>380</v>
+        <v>531</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>358</v>
@@ -4657,24 +4651,24 @@
         <v>360</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>472</v>
+        <v>533</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>358</v>
@@ -4686,24 +4680,24 @@
         <v>360</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>358</v>
@@ -4715,24 +4709,24 @@
         <v>360</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>358</v>
@@ -4744,24 +4738,24 @@
         <v>360</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>358</v>
@@ -4773,24 +4767,24 @@
         <v>360</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>358</v>
@@ -4802,24 +4796,24 @@
         <v>360</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>358</v>
@@ -4831,24 +4825,24 @@
         <v>360</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>358</v>
@@ -4860,24 +4854,24 @@
         <v>360</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>358</v>
@@ -4889,21 +4883,19 @@
         <v>360</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>408</v>
-      </c>
+      <c r="A11" s="37"/>
       <c r="B11" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>358</v>
@@ -4915,10 +4907,10 @@
         <v>360</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -4947,33 +4939,33 @@
         <v>363</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="36" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="36" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="36" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -5010,145 +5002,145 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B4" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B5" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B8" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B9" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B10" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B12" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B13" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B14" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -5831,7 +5823,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5887,7 +5879,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -6031,7 +6023,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="43" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6042,7 +6034,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="48" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6074,7 +6066,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6083,7 +6075,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="49"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6123,7 +6115,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="47" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6144,7 +6136,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="48" t="s">
+      <c r="K33" s="47" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6164,7 +6156,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6183,7 +6175,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="48"/>
+      <c r="K34" s="47"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6204,7 +6196,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="47" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6225,7 +6217,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="48" t="s">
+      <c r="K36" s="47" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6245,7 +6237,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6264,7 +6256,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="48"/>
+      <c r="K37" s="47"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6282,7 +6274,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="48" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6300,7 +6292,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="48" t="s">
+      <c r="K39" s="47" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6320,7 +6312,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6336,7 +6328,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="48"/>
+      <c r="K40" s="47"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6354,7 +6346,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="43" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6389,7 +6381,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6434,7 +6426,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="42" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6487,7 +6479,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -6538,7 +6530,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="43" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6603,7 +6595,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -6667,6 +6659,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -6676,11 +6673,6 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
Final code added for https://veriday.atlassian.net/browse/ETI-6 ticket
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A5A909-E574-4C46-B293-A5865722022C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F77989E-21F9-4F11-BB56-776729546589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,10 @@
     <sheet name="CreateUser" sheetId="2" r:id="rId3"/>
     <sheet name="CreateNewForm" sheetId="9" r:id="rId4"/>
     <sheet name="CreateTeamUser" sheetId="5" r:id="rId5"/>
-    <sheet name="SearchUser" sheetId="6" r:id="rId6"/>
-    <sheet name="NewEventDetails" sheetId="7" r:id="rId7"/>
-    <sheet name="Branch" sheetId="4" r:id="rId8"/>
+    <sheet name="NewGroup" sheetId="10" r:id="rId6"/>
+    <sheet name="SearchUser" sheetId="6" r:id="rId7"/>
+    <sheet name="NewEventDetails" sheetId="7" r:id="rId8"/>
+    <sheet name="Branch" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="537">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1635,6 +1636,9 @@
   </si>
   <si>
     <t>James</t>
+  </si>
+  <si>
+    <t>AutomationGroup</t>
   </si>
 </sst>
 </file>
@@ -1855,17 +1859,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1873,17 +1871,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2194,7 +2198,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2208,7 +2212,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -2368,13 +2372,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="44"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2387,7 +2391,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2654,7 +2658,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="45"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2687,7 +2691,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="45"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3032,14 +3036,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3577,13 +3581,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3611,13 +3615,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3645,6 +3649,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3661,11 +3670,6 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -4587,7 +4591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02286501-8169-47C9-B0C1-20840CFA8C0B}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4921,6 +4925,35 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28877364-3A8C-400C-A086-72B83FEB2E27}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76A90F2-FEBC-495D-96DD-9CDE989D1767}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -4974,7 +5007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC62FD-4EDF-4588-A45B-85367A874BBC}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -5152,7 +5185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH52"/>
   <sheetViews>
@@ -5823,7 +5856,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5879,7 +5912,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -6023,7 +6056,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="40" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6034,7 +6067,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="49" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6066,7 +6099,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6075,7 +6108,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="48"/>
+      <c r="F31" s="49"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6115,7 +6148,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="48" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6136,7 +6169,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="47" t="s">
+      <c r="K33" s="48" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6156,7 +6189,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6175,7 +6208,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="47"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6196,7 +6229,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="48" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6217,7 +6250,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="47" t="s">
+      <c r="K36" s="48" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6237,7 +6270,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6256,7 +6289,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="47"/>
+      <c r="K37" s="48"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6274,7 +6307,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="49" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6292,7 +6325,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="47" t="s">
+      <c r="K39" s="48" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6312,7 +6345,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6328,7 +6361,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="47"/>
+      <c r="K40" s="48"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6346,7 +6379,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="40" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6381,7 +6414,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6426,7 +6459,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="45" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6479,7 +6512,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -6530,7 +6563,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="40" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6595,7 +6628,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -6659,11 +6692,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -6673,6 +6701,11 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
final code added for https://veriday.atlassian.net/browse/ETI-6
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F77989E-21F9-4F11-BB56-776729546589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E945A0-6375-4192-AACB-4F4882EBDD67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="547">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1639,13 +1639,54 @@
   </si>
   <si>
     <t>AutomationGroup</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5580</t>
+    </r>
+  </si>
+  <si>
+    <t>Explorer Dr, Mississauga</t>
+  </si>
+  <si>
+    <t>Mississauga</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>L4W</t>
+  </si>
+  <si>
+    <t>Branch/RegionAddressLine1</t>
+  </si>
+  <si>
+    <t>Branch/RegionAddressLine2</t>
+  </si>
+  <si>
+    <t>Branch/Region-City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1742,6 +1783,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1782,7 +1836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1859,11 +1913,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1871,17 +1931,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1889,6 +1940,11 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2198,7 +2254,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2212,7 +2268,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
+      <c r="A2" s="43"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -2372,13 +2428,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="40"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2391,7 +2447,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2658,7 +2714,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="42"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2691,7 +2747,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="42"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3036,14 +3092,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3581,13 +3637,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3615,13 +3671,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3649,11 +3705,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3670,6 +3721,11 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -4926,25 +4982,63 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28877364-3A8C-400C-A086-72B83FEB2E27}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>536</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>538</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>543</v>
+      </c>
+      <c r="G2" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -5856,7 +5950,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -5912,7 +6006,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -6056,7 +6150,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="43" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6067,7 +6161,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="48" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6099,7 +6193,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6108,7 +6202,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="49"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6148,7 +6242,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="47" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6169,7 +6263,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="48" t="s">
+      <c r="K33" s="47" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6189,7 +6283,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6208,7 +6302,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="48"/>
+      <c r="K34" s="47"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6229,7 +6323,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="47" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6250,7 +6344,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="48" t="s">
+      <c r="K36" s="47" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6270,7 +6364,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6289,7 +6383,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="48"/>
+      <c r="K37" s="47"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6307,7 +6401,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="48" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6325,7 +6419,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="48" t="s">
+      <c r="K39" s="47" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6345,7 +6439,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6361,7 +6455,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="48"/>
+      <c r="K40" s="47"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6379,7 +6473,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="43" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6414,7 +6508,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6459,7 +6553,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="42" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6512,7 +6606,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -6563,7 +6657,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="43" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6628,7 +6722,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -6692,6 +6786,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -6701,11 +6800,6 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
code modified for creae region & branch
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E945A0-6375-4192-AACB-4F4882EBDD67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210B85E-C709-415F-B19C-21F725868836}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="550">
   <si>
     <t>HeadOffice</t>
   </si>
@@ -1680,6 +1680,15 @@
   </si>
   <si>
     <t>Branch/Region-City</t>
+  </si>
+  <si>
+    <t>RegionName</t>
+  </si>
+  <si>
+    <t>AutomationRegion</t>
+  </si>
+  <si>
+    <t>AutomationBranch</t>
   </si>
 </sst>
 </file>
@@ -1913,17 +1922,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1931,8 +1936,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1940,11 +1954,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2254,7 +2263,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2268,7 +2277,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
+      <c r="A2" s="42"/>
       <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
@@ -2428,13 +2437,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="46"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="46"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2447,7 +2456,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2714,7 +2723,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="47"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2747,7 +2756,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="47"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3092,14 +3101,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3127,13 +3136,13 @@
     </row>
     <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -3161,13 +3170,13 @@
     </row>
     <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -3195,13 +3204,13 @@
     </row>
     <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -3229,13 +3238,13 @@
     </row>
     <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -3263,13 +3272,13 @@
     </row>
     <row r="49" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -3297,13 +3306,13 @@
     </row>
     <row r="50" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -3331,13 +3340,13 @@
     </row>
     <row r="51" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -3365,13 +3374,13 @@
     </row>
     <row r="52" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="41"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -3399,13 +3408,13 @@
     </row>
     <row r="53" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -3433,13 +3442,13 @@
     </row>
     <row r="54" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -3501,13 +3510,13 @@
     </row>
     <row r="56" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3535,13 +3544,13 @@
     </row>
     <row r="57" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="B57" s="41"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -3569,13 +3578,13 @@
     </row>
     <row r="58" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="B58" s="41"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="41"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -3603,13 +3612,13 @@
     </row>
     <row r="59" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
-      <c r="B59" s="41"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="41"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -3705,6 +3714,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3721,11 +3735,6 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
@@ -4982,10 +4991,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28877364-3A8C-400C-A086-72B83FEB2E27}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,9 +5002,11 @@
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -5017,15 +5028,21 @@
       <c r="G1" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>536</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="40" t="s">
         <v>538</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="41" t="s">
         <v>539</v>
       </c>
       <c r="D2" t="s">
@@ -5034,11 +5051,17 @@
       <c r="E2" t="s">
         <v>541</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="41" t="s">
         <v>543</v>
       </c>
       <c r="G2" t="s">
         <v>542</v>
+      </c>
+      <c r="H2" t="s">
+        <v>548</v>
+      </c>
+      <c r="I2" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -5300,7 +5323,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -5404,7 +5427,7 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="6" t="s">
         <v>188</v>
       </c>
@@ -6075,7 +6098,7 @@
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="48" t="s">
         <v>198</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -6107,7 +6130,7 @@
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="6" t="s">
         <v>203</v>
       </c>
@@ -6150,7 +6173,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="42" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6161,7 +6184,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="51" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6193,7 +6216,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6202,7 +6225,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="48"/>
+      <c r="F31" s="51"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6242,7 +6265,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="50" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6263,7 +6286,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="47" t="s">
+      <c r="K33" s="50" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6283,7 +6306,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6302,7 +6325,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="47"/>
+      <c r="K34" s="50"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6323,7 +6346,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="50" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6344,7 +6367,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="47" t="s">
+      <c r="K36" s="50" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6364,7 +6387,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6383,7 +6406,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="47"/>
+      <c r="K37" s="50"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6401,7 +6424,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="51" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6419,7 +6442,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="47" t="s">
+      <c r="K39" s="50" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6439,7 +6462,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6455,7 +6478,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="47"/>
+      <c r="K40" s="50"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6473,7 +6496,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="42" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6508,7 +6531,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
+      <c r="A44" s="42"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6553,7 +6576,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="47" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6606,7 +6629,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -6657,7 +6680,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="42" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6722,7 +6745,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -6786,11 +6809,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -6800,6 +6818,11 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
extent report 5 code added
</commit_message>
<xml_diff>
--- a/source/TestData.xlsx
+++ b/source/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210B85E-C709-415F-B19C-21F725868836}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73209C1F-B7A2-45D2-A5FE-EE8E9E1C15CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1924,11 +1924,17 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1936,23 +1942,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2237,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,7 +2263,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2277,8 +2277,8 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="23" t="s">
         <v>351</v>
       </c>
       <c r="C2" s="33" t="s">
@@ -2437,13 +2437,13 @@
       <c r="AE9" s="6"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="42"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="42"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2456,7 +2456,7 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2723,7 +2723,7 @@
       <c r="AF31" s="6"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="44"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2756,7 +2756,7 @@
       <c r="AF32" s="6"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="44"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3101,14 +3101,14 @@
       <c r="AF43" s="6"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -3646,13 +3646,13 @@
     </row>
     <row r="60" spans="1:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3680,13 +3680,13 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3714,11 +3714,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B61:H61"/>
@@ -3735,12 +3730,18 @@
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@12345" xr:uid="{07323420-B809-480C-A764-185C7B030B8F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C6A108B5-EAD9-4CDA-939B-8D513990E099}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4993,7 +4994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28877364-3A8C-400C-A086-72B83FEB2E27}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -5973,7 +5974,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="51" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -6029,7 +6030,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
@@ -6173,7 +6174,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="45" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6184,7 +6185,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="51" t="s">
+      <c r="F30" s="50" t="s">
         <v>281</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -6216,7 +6217,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="6" t="s">
         <v>279</v>
       </c>
@@ -6225,7 +6226,7 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="51"/>
+      <c r="F31" s="50"/>
       <c r="G31" s="6" t="s">
         <v>282</v>
       </c>
@@ -6265,7 +6266,7 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="49" t="s">
         <v>227</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -6286,7 +6287,7 @@
       <c r="G33" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K33" s="50" t="s">
+      <c r="K33" s="49" t="s">
         <v>236</v>
       </c>
       <c r="L33" s="31" t="s">
@@ -6306,7 +6307,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="6" t="s">
         <v>288</v>
       </c>
@@ -6325,7 +6326,7 @@
       <c r="G34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="50"/>
+      <c r="K34" s="49"/>
       <c r="L34" s="6" t="s">
         <v>291</v>
       </c>
@@ -6346,7 +6347,7 @@
       <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="49" t="s">
         <v>232</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -6367,7 +6368,7 @@
       <c r="G36" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="K36" s="50" t="s">
+      <c r="K36" s="49" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="31" t="s">
@@ -6387,7 +6388,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="6" t="s">
         <v>289</v>
       </c>
@@ -6406,7 +6407,7 @@
       <c r="G37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="50"/>
+      <c r="K37" s="49"/>
       <c r="L37" s="6" t="s">
         <v>224</v>
       </c>
@@ -6424,7 +6425,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="50" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -6442,7 +6443,7 @@
       <c r="F39" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="K39" s="50" t="s">
+      <c r="K39" s="49" t="s">
         <v>246</v>
       </c>
       <c r="L39" s="31" t="s">
@@ -6462,7 +6463,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="6" t="s">
         <v>290</v>
       </c>
@@ -6478,7 +6479,7 @@
       <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K40" s="50"/>
+      <c r="K40" s="49"/>
       <c r="L40" s="6" t="s">
         <v>292</v>
       </c>
@@ -6496,7 +6497,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="45" t="s">
         <v>294</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -6531,7 +6532,7 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="6" t="s">
         <v>307</v>
       </c>
@@ -6576,7 +6577,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="44" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6629,7 +6630,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="6" t="s">
         <v>308</v>
       </c>
@@ -6680,7 +6681,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="45" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6745,7 +6746,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
+      <c r="A52" s="45"/>
       <c r="B52" s="6" t="s">
         <v>327</v>
       </c>
@@ -6809,6 +6810,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A26:A27"/>
@@ -6818,11 +6824,6 @@
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>